<commit_message>
add reinforced random walk
</commit_message>
<xml_diff>
--- a/evaluation/best_results.xlsx
+++ b/evaluation/best_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lguan/Documents/Study/ASU/CSE 575 Statistical Machine Learning/Graph-Embedding-Algorithms/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77603E4-EBFE-E647-A5AA-ACDEFA4B7B2B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F330D2B-DD7C-0242-9511-8953156010EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35560" yWindow="2200" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{BAD8D954-232B-8740-B009-5BF2A445F6DD}"/>
+    <workbookView xWindow="-34960" yWindow="1720" windowWidth="28040" windowHeight="17440" xr2:uid="{BAD8D954-232B-8740-B009-5BF2A445F6DD}"/>
   </bookViews>
   <sheets>
     <sheet name="blog-catalog" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="16">
   <si>
     <t>test_set_size</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>simple_random_walk-1574361871.648308</t>
+  </si>
+  <si>
+    <t>temperature-walk</t>
+  </si>
+  <si>
+    <t>bfs-dfs-combined</t>
   </si>
 </sst>
 </file>
@@ -1951,7 +1957,7 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
@@ -1960,123 +1966,6 @@
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>biased-walk-dfs</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>ppi!$E$5:$M$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>ppi!$E$6:$M$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
-                <c:pt idx="0">
-                  <c:v>0.18740903372505099</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.19608284782853799</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.194621609149664</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.187617494433924</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.182722915314632</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.16436696179662399</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.163362166510408</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.15778821261294401</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.13848698017328401</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4AC1-9942-8E9C-EEDB4366A260}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>ppi!$D$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>approximate-dfs</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2143,36 +2032,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ppi!$E$7:$M$7</c:f>
+              <c:f>ppi!$E$6:$M$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.21128921065397299</c:v>
+                  <c:v>0.18740903372505099</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.18486176758540601</c:v>
+                  <c:v>0.19608284782853799</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.17494997755872199</c:v>
+                  <c:v>0.194621609149664</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.177365451727166</c:v>
+                  <c:v>0.187617494433924</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.18033241607914899</c:v>
+                  <c:v>0.182722915314632</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.17847259292790599</c:v>
+                  <c:v>0.16436696179662399</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.16119827745865301</c:v>
+                  <c:v>0.163362166510408</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.16442479541701599</c:v>
+                  <c:v>0.15778821261294401</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.13766349284284499</c:v>
+                  <c:v>0.13848698017328401</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2186,14 +2075,14 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>ppi!$D$8</c:f>
+              <c:f>ppi!$D$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>approximate-bfs</c:v>
+                  <c:v>approximate-dfs</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2260,36 +2149,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ppi!$E$8:$M$8</c:f>
+              <c:f>ppi!$E$7:$M$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.206249360331409</c:v>
+                  <c:v>0.21128921065397299</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.190456967780472</c:v>
+                  <c:v>0.18486176758540601</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.17784078787455701</c:v>
+                  <c:v>0.17494997755872199</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17767776089592499</c:v>
+                  <c:v>0.177365451727166</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.17333344468290099</c:v>
+                  <c:v>0.18033241607914899</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.16021387806172699</c:v>
+                  <c:v>0.17847259292790599</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.15471652381366</c:v>
+                  <c:v>0.16119827745865301</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.155397980859691</c:v>
+                  <c:v>0.16442479541701599</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.13190574058318599</c:v>
+                  <c:v>0.13766349284284499</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2303,14 +2192,14 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>ppi!$D$9</c:f>
+              <c:f>ppi!$D$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>node2vec-walk</c:v>
+                  <c:v>approximate-bfs</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2377,36 +2266,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ppi!$E$9:$M$9</c:f>
+              <c:f>ppi!$E$8:$M$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.206815339127329</c:v>
+                  <c:v>0.206249360331409</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.184286166895194</c:v>
+                  <c:v>0.190456967780472</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.17909449434838101</c:v>
+                  <c:v>0.17784078787455701</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17419145732954999</c:v>
+                  <c:v>0.17767776089592499</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.17350906403171301</c:v>
+                  <c:v>0.17333344468290099</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.16756113272444001</c:v>
+                  <c:v>0.16021387806172699</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.15849486988842201</c:v>
+                  <c:v>0.15471652381366</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.159923900316845</c:v>
+                  <c:v>0.155397980859691</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.137083896713628</c:v>
+                  <c:v>0.13190574058318599</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2420,14 +2309,14 @@
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
-          <c:order val="4"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>ppi!$D$10</c:f>
+              <c:f>ppi!$D$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>simple-random-walk</c:v>
+                  <c:v>node2vec-walk</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2494,36 +2383,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ppi!$E$10:$M$10</c:f>
+              <c:f>ppi!$E$9:$M$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.19786588894149301</c:v>
+                  <c:v>0.206815339127329</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.192302099891173</c:v>
+                  <c:v>0.184286166895194</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.18936469743414</c:v>
+                  <c:v>0.17909449434838101</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.18850384706266199</c:v>
+                  <c:v>0.17419145732954999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.174504762361649</c:v>
+                  <c:v>0.17350906403171301</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.16999644324961899</c:v>
+                  <c:v>0.16756113272444001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.16200666078503501</c:v>
+                  <c:v>0.15849486988842201</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.16151807535526599</c:v>
+                  <c:v>0.159923900316845</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.141141831678887</c:v>
+                  <c:v>0.137083896713628</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2532,6 +2421,246 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-4AC1-9942-8E9C-EEDB4366A260}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ppi!$D$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>simple-random-walk</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ppi!$E$5:$M$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ppi!$E$10:$M$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.19786588894149301</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.192302099891173</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.18936469743414</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.18850384706266199</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.174504762361649</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16999644324961899</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.16200666078503501</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.16151807535526599</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.141141831678887</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-4AC1-9942-8E9C-EEDB4366A260}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ppi!$D$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>temperature-walk</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ppi!$E$5:$M$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ppi!$E$11:$M$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.20848719302855101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.19573537936042401</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17911386181807501</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17205512130384601</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.17408323654886801</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16906742617693901</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.159036808198288</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.15445238097868899</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.13650668026857801</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-4AC1-9942-8E9C-EEDB4366A260}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3044,7 +3173,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E305-8646-A85D-81CC63DE7C30}"/>
+              <c16:uniqueId val="{00000006-E305-8646-A85D-81CC63DE7C30}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3161,7 +3290,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-E305-8646-A85D-81CC63DE7C30}"/>
+              <c16:uniqueId val="{00000007-E305-8646-A85D-81CC63DE7C30}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3278,7 +3407,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-E305-8646-A85D-81CC63DE7C30}"/>
+              <c16:uniqueId val="{00000008-E305-8646-A85D-81CC63DE7C30}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3395,7 +3524,124 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-E305-8646-A85D-81CC63DE7C30}"/>
+              <c16:uniqueId val="{00000009-E305-8646-A85D-81CC63DE7C30}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ppi!$D$31</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>temperature-walk</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ppi!$E$25:$M$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ppi!$E$31:$M$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.25266362252663599</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.22842261904761901</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.21552150271873499</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.20716981132075499</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.205019655276686</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.20272658419591</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.190979715148899</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.183320668693009</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.173002196316945</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-E305-8646-A85D-81CC63DE7C30}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6226,10 +6472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F570716-1562-E44E-8EDB-72005B36B087}">
-  <dimension ref="B4:L30"/>
+  <dimension ref="B4:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="88" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="D19" zoomScale="144" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6453,6 +6699,38 @@
         <v>0.16155166268211699</v>
       </c>
     </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.268375227971206</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.27456415267086998</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.27206243713349598</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.271743118185583</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.26658620540975397</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.25967961466037898</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0.24532227078149499</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0.223624588565283</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0.192192241365784</v>
+      </c>
+    </row>
     <row r="24" spans="2:12" ht="24" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
         <v>4</v>
@@ -6666,6 +6944,38 @@
       </c>
       <c r="L30" s="2">
         <v>0.34316436251920102</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.41637508747375801</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0.41555242786769903</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.41563304469927498</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.41332403208929203</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0.40886217500698901</v>
+      </c>
+      <c r="I31" s="2">
+        <v>0.40104166666666702</v>
+      </c>
+      <c r="J31" s="2">
+        <v>0.39028991262907098</v>
+      </c>
+      <c r="K31" s="2">
+        <v>0.37346267105491099</v>
+      </c>
+      <c r="L31" s="2">
+        <v>0.35660522273425499</v>
       </c>
     </row>
   </sheetData>
@@ -6677,10 +6987,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAEA373-FC8B-FF43-890F-32ABE335373B}">
-  <dimension ref="C4:M30"/>
+  <dimension ref="C4:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="92" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView zoomScale="68" workbookViewId="0">
+      <selection activeCell="R44" sqref="R44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6904,8 +7214,37 @@
         <v>0.141141831678887</v>
       </c>
     </row>
-    <row r="12" spans="3:13" x14ac:dyDescent="0.2">
-      <c r="E12" s="2"/>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.20848719302855101</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0.19573537936042401</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.17911386181807501</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0.17205512130384601</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.17408323654886801</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0.16906742617693901</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0.159036808198288</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0.15445238097868899</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0.13650668026857801</v>
+      </c>
     </row>
     <row r="24" spans="3:13" ht="24" x14ac:dyDescent="0.3">
       <c r="C24" s="3" t="s">
@@ -7120,6 +7459,38 @@
       </c>
       <c r="M30" s="2">
         <v>0.17671904037844199</v>
+      </c>
+    </row>
+    <row r="31" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0.25266362252663599</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.22842261904761901</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.21552150271873499</v>
+      </c>
+      <c r="H31" s="2">
+        <v>0.20716981132075499</v>
+      </c>
+      <c r="I31" s="2">
+        <v>0.205019655276686</v>
+      </c>
+      <c r="J31" s="2">
+        <v>0.20272658419591</v>
+      </c>
+      <c r="K31" s="2">
+        <v>0.190979715148899</v>
+      </c>
+      <c r="L31" s="2">
+        <v>0.183320668693009</v>
+      </c>
+      <c r="M31" s="2">
+        <v>0.173002196316945</v>
       </c>
     </row>
   </sheetData>

</xml_diff>